<commit_message>
REF/SM: Generate settings for LS3 cavity tuning.
</commit_message>
<xml_diff>
--- a/phantasy_apps/settings_manager/contrib/settings_support_cavity_tuning/ARR05_86Kr34_magnet_setting_ver20210422.xlsx
+++ b/phantasy_apps/settings_manager/contrib/settings_support_cavity_tuning/ARR05_86Kr34_magnet_setting_ver20210422.xlsx
@@ -326,227 +326,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:BR4"/>
+  <dimension ref="A2:BS4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.55"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="T2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="U2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="X2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Z2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="AA2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AB2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AC2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AD2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AE2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AF2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="0" t="s">
+      <c r="AG2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="0" t="s">
+      <c r="AH2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="0" t="s">
+      <c r="AI2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="0" t="s">
+      <c r="AJ2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="0" t="s">
+      <c r="AK2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="AK2" s="0" t="s">
+      <c r="AL2" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="AL2" s="0" t="s">
+      <c r="AM2" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="AM2" s="0" t="s">
+      <c r="AN2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="AN2" s="0" t="s">
+      <c r="AO2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="AO2" s="0" t="s">
+      <c r="AP2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="AP2" s="0" t="s">
+      <c r="AQ2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="AQ2" s="0" t="s">
+      <c r="AR2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="0" t="s">
+      <c r="AS2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="AS2" s="0" t="s">
+      <c r="AT2" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AT2" s="0" t="s">
+      <c r="AU2" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="AU2" s="0" t="s">
+      <c r="AV2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="AV2" s="0" t="s">
+      <c r="AW2" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="AW2" s="0" t="s">
+      <c r="AX2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" s="0" t="s">
+      <c r="AY2" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="AY2" s="0" t="s">
+      <c r="AZ2" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="AZ2" s="0" t="s">
+      <c r="BA2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="BA2" s="0" t="s">
+      <c r="BB2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="BB2" s="0" t="s">
+      <c r="BC2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="BC2" s="0" t="s">
+      <c r="BD2" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="BD2" s="0" t="s">
+      <c r="BE2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="BE2" s="0" t="s">
+      <c r="BF2" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="BF2" s="0" t="s">
+      <c r="BG2" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="BG2" s="0" t="s">
+      <c r="BH2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="BH2" s="0" t="s">
+      <c r="BI2" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="BI2" s="0" t="s">
+      <c r="BJ2" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="BJ2" s="0" t="s">
+      <c r="BK2" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="BK2" s="0" t="s">
+      <c r="BL2" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="BL2" s="0" t="s">
+      <c r="BM2" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="BM2" s="0" t="s">
+      <c r="BN2" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="BN2" s="0" t="s">
+      <c r="BO2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="BO2" s="0" t="s">
+      <c r="BP2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="BP2" s="0" t="s">
+      <c r="BQ2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="BQ2" s="0" t="s">
+      <c r="BR2" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="BR2" s="0" t="s">
+      <c r="BS2" s="0" t="s">
         <v>68</v>
       </c>
     </row>
@@ -554,211 +555,211 @@
       <c r="A3" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>212.49</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>37.9840095969145</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>17.4588759616225</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>62.6561800431234</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>47.4099597934764</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>140.681795552455</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>217.996145497324</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>199.423469257642</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="L3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>202.658714417342</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>140.681795552455</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>140.681795552455</v>
       </c>
       <c r="O3" s="0" t="n">
+        <v>140.681795552455</v>
+      </c>
+      <c r="P3" s="0" t="n">
         <v>202.658714417342</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="Q3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="R3" s="0" t="n">
         <v>199.423469257642</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="S3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="T3" s="0" t="n">
         <v>217.996145497324</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="U3" s="0" t="n">
         <v>140.681795552455</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="V3" s="0" t="n">
         <v>11.8924878028147</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="W3" s="0" t="n">
         <v>4.34725256118906</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="X3" s="0" t="n">
         <v>72.2563674932777</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="Y3" s="0" t="n">
         <v>56.1617855839944</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Z3" s="0" t="n">
         <v>87.9974649658536</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="AA3" s="0" t="n">
         <v>98.6972694388393</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AB3" s="0" t="n">
         <v>71.9079045873688</v>
       </c>
-      <c r="AB3" s="0" t="n">
+      <c r="AC3" s="0" t="n">
         <v>67.3727656512644</v>
       </c>
-      <c r="AC3" s="0" t="n">
+      <c r="AD3" s="0" t="n">
         <v>72.0902908863951</v>
       </c>
-      <c r="AD3" s="0" t="n">
+      <c r="AE3" s="0" t="n">
         <v>69.21764306191</v>
       </c>
-      <c r="AE3" s="0" t="n">
+      <c r="AF3" s="0" t="n">
         <v>68.0148309061115</v>
       </c>
-      <c r="AF3" s="0" t="n">
+      <c r="AG3" s="0" t="n">
         <v>66.7142082033668</v>
       </c>
-      <c r="AG3" s="0" t="n">
+      <c r="AH3" s="0" t="n">
         <v>65.2595517059524</v>
       </c>
-      <c r="AH3" s="0" t="n">
+      <c r="AI3" s="0" t="n">
         <v>66.864814664667</v>
       </c>
-      <c r="AI3" s="0" t="n">
+      <c r="AJ3" s="0" t="n">
         <v>67.6849674730809</v>
       </c>
-      <c r="AJ3" s="0" t="n">
+      <c r="AK3" s="0" t="n">
         <v>110.019008434845</v>
       </c>
-      <c r="AK3" s="0" t="n">
+      <c r="AL3" s="0" t="n">
         <v>118.726567540819</v>
       </c>
-      <c r="AL3" s="0" t="n">
+      <c r="AM3" s="0" t="n">
         <v>95.5365100752224</v>
       </c>
-      <c r="AM3" s="0" t="n">
+      <c r="AN3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="AN3" s="0" t="n">
+      <c r="AO3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="AO3" s="0" t="n">
+      <c r="AP3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="AP3" s="0" t="n">
+      <c r="AQ3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="AQ3" s="0" t="n">
+      <c r="AR3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="AR3" s="0" t="n">
+      <c r="AS3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="AS3" s="0" t="n">
+      <c r="AT3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="AT3" s="0" t="n">
+      <c r="AU3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="AU3" s="0" t="n">
+      <c r="AV3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="AV3" s="0" t="n">
+      <c r="AW3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="AW3" s="0" t="n">
+      <c r="AX3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="AX3" s="0" t="n">
+      <c r="AY3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="AY3" s="0" t="n">
+      <c r="AZ3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="AZ3" s="0" t="n">
+      <c r="BA3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="BA3" s="0" t="n">
+      <c r="BB3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="BB3" s="0" t="n">
+      <c r="BC3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="BC3" s="0" t="n">
+      <c r="BD3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="BD3" s="0" t="n">
+      <c r="BE3" s="0" t="n">
         <v>55.48824929381</v>
       </c>
-      <c r="BE3" s="0" t="n">
+      <c r="BF3" s="0" t="n">
         <v>75.2546259946389</v>
       </c>
-      <c r="BF3" s="0" t="n">
+      <c r="BG3" s="0" t="n">
         <v>60.1754872409247</v>
       </c>
-      <c r="BG3" s="0" t="n">
+      <c r="BH3" s="0" t="n">
         <v>81.6115718337827</v>
       </c>
-      <c r="BH3" s="0" t="n">
+      <c r="BI3" s="0" t="n">
         <v>60.1754872409247</v>
       </c>
-      <c r="BI3" s="0" t="n">
+      <c r="BJ3" s="0" t="n">
         <v>102.750609914994</v>
       </c>
-      <c r="BJ3" s="0" t="n">
+      <c r="BK3" s="0" t="n">
         <v>104.769156579623</v>
       </c>
-      <c r="BK3" s="0" t="n">
+      <c r="BL3" s="0" t="n">
         <v>130.49700316211</v>
       </c>
-      <c r="BL3" s="0" t="n">
+      <c r="BM3" s="0" t="n">
         <v>104.907455976035</v>
       </c>
-      <c r="BM3" s="0" t="n">
+      <c r="BN3" s="0" t="n">
         <v>80.9559178758952</v>
       </c>
-      <c r="BN3" s="0" t="n">
+      <c r="BO3" s="0" t="n">
         <v>89.5633341169019</v>
       </c>
-      <c r="BO3" s="0" t="n">
+      <c r="BP3" s="0" t="n">
         <v>76.3563370164379</v>
       </c>
-      <c r="BP3" s="0" t="n">
+      <c r="BQ3" s="0" t="n">
         <v>79.2679030186519</v>
       </c>
-      <c r="BQ3" s="0" t="n">
+      <c r="BR3" s="0" t="n">
         <v>142.229204805764</v>
       </c>
-      <c r="BR3" s="0" t="n">
+      <c r="BS3" s="0" t="n">
         <v>70.6806001436464</v>
       </c>
     </row>
@@ -766,211 +767,211 @@
       <c r="A4" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>182.12</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>37.9840095969145</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>17.4588759616225</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>62.6561800431234</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>47.4099597934764</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>140.681795552455</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>217.996145497324</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>199.423469257642</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="L4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="M4" s="0" t="n">
         <v>202.658714417342</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>140.681795552455</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>140.681795552455</v>
       </c>
       <c r="O4" s="0" t="n">
+        <v>140.681795552455</v>
+      </c>
+      <c r="P4" s="0" t="n">
         <v>202.658714417342</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="Q4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="R4" s="0" t="n">
         <v>199.423469257642</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="S4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="T4" s="0" t="n">
         <v>217.996145497324</v>
       </c>
-      <c r="T4" s="0" t="n">
+      <c r="U4" s="0" t="n">
         <v>140.681795552455</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="V4" s="0" t="n">
         <v>11.8924878028147</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="W4" s="0" t="n">
         <v>4.34725256118906</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="X4" s="0" t="n">
         <v>72.2563674932777</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="Y4" s="0" t="n">
         <v>56.1617855839944</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Z4" s="0" t="n">
         <v>87.9974649658536</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="AA4" s="0" t="n">
         <v>98.6972694388393</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AB4" s="0" t="n">
         <v>71.9079045873688</v>
       </c>
-      <c r="AB4" s="0" t="n">
+      <c r="AC4" s="0" t="n">
         <v>67.3727656512644</v>
       </c>
-      <c r="AC4" s="0" t="n">
+      <c r="AD4" s="0" t="n">
         <v>72.6351612687348</v>
       </c>
-      <c r="AD4" s="0" t="n">
+      <c r="AE4" s="0" t="n">
         <v>70.7787621684602</v>
       </c>
-      <c r="AE4" s="0" t="n">
+      <c r="AF4" s="0" t="n">
         <v>70.5580139535345</v>
       </c>
-      <c r="AF4" s="0" t="n">
+      <c r="AG4" s="0" t="n">
         <v>70.188383136754</v>
       </c>
-      <c r="AG4" s="0" t="n">
+      <c r="AH4" s="0" t="n">
         <v>69.60644669311</v>
       </c>
-      <c r="AH4" s="0" t="n">
+      <c r="AI4" s="0" t="n">
         <v>72.2806634076329</v>
       </c>
-      <c r="AI4" s="0" t="n">
+      <c r="AJ4" s="0" t="n">
         <v>73.6505312325835</v>
       </c>
-      <c r="AJ4" s="0" t="n">
+      <c r="AK4" s="0" t="n">
         <v>119.715776182224</v>
       </c>
-      <c r="AK4" s="0" t="n">
+      <c r="AL4" s="0" t="n">
         <v>129.190795198066</v>
       </c>
-      <c r="AL4" s="0" t="n">
+      <c r="AM4" s="0" t="n">
         <v>103.956830915899</v>
       </c>
-      <c r="AM4" s="0" t="n">
+      <c r="AN4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="AN4" s="0" t="n">
+      <c r="AO4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="AO4" s="0" t="n">
+      <c r="AP4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="AP4" s="0" t="n">
+      <c r="AQ4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="AQ4" s="0" t="n">
+      <c r="AR4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="AR4" s="0" t="n">
+      <c r="AS4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="AS4" s="0" t="n">
+      <c r="AT4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="AT4" s="0" t="n">
+      <c r="AU4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="AU4" s="0" t="n">
+      <c r="AV4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="AV4" s="0" t="n">
+      <c r="AW4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="AW4" s="0" t="n">
+      <c r="AX4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="AX4" s="0" t="n">
+      <c r="AY4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="AY4" s="0" t="n">
+      <c r="AZ4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="AZ4" s="0" t="n">
+      <c r="BA4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="BA4" s="0" t="n">
+      <c r="BB4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="BB4" s="0" t="n">
+      <c r="BC4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="BC4" s="0" t="n">
+      <c r="BD4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="BD4" s="0" t="n">
+      <c r="BE4" s="0" t="n">
         <v>60.3788284197741</v>
       </c>
-      <c r="BE4" s="0" t="n">
+      <c r="BF4" s="0" t="n">
         <v>81.8873582885134</v>
       </c>
-      <c r="BF4" s="0" t="n">
+      <c r="BG4" s="0" t="n">
         <v>65.4791864122016</v>
       </c>
-      <c r="BG4" s="0" t="n">
+      <c r="BH4" s="0" t="n">
         <v>88.8045875574188</v>
       </c>
-      <c r="BH4" s="0" t="n">
+      <c r="BI4" s="0" t="n">
         <v>65.4791864122016</v>
       </c>
-      <c r="BI4" s="0" t="n">
+      <c r="BJ4" s="0" t="n">
         <v>111.806761342111</v>
       </c>
-      <c r="BJ4" s="0" t="n">
+      <c r="BK4" s="0" t="n">
         <v>114.003217065116</v>
       </c>
-      <c r="BK4" s="0" t="n">
+      <c r="BL4" s="0" t="n">
         <v>141.998644100288</v>
       </c>
-      <c r="BL4" s="0" t="n">
+      <c r="BM4" s="0" t="n">
         <v>114.153705783589</v>
       </c>
-      <c r="BM4" s="0" t="n">
+      <c r="BN4" s="0" t="n">
         <v>88.0911460931473</v>
       </c>
-      <c r="BN4" s="0" t="n">
+      <c r="BO4" s="0" t="n">
         <v>97.4571959319425</v>
       </c>
-      <c r="BO4" s="0" t="n">
+      <c r="BP4" s="0" t="n">
         <v>83.0861710389599</v>
       </c>
-      <c r="BP4" s="0" t="n">
+      <c r="BQ4" s="0" t="n">
         <v>86.2543543267346</v>
       </c>
-      <c r="BQ4" s="0" t="n">
+      <c r="BR4" s="0" t="n">
         <v>154.764889189</v>
       </c>
-      <c r="BR4" s="0" t="n">
+      <c r="BS4" s="0" t="n">
         <v>76.9101905897751</v>
       </c>
     </row>

</xml_diff>